<commit_message>
tach data push 3/15/21
</commit_message>
<xml_diff>
--- a/Single_Motor_2018_08_08_02_Tacho .xlsx
+++ b/Single_Motor_2018_08_08_02_Tacho .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timmy\Documents\Aero Reasearch\JR3-vs-ATI-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBB08A4-CD4F-4D7B-9B4D-66928E1EB531}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560FBF3B-CBDF-47A7-A24E-875146E9DCB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>CONTINUOUS_MODE</t>
   </si>
@@ -104,10 +104,16 @@
     <t xml:space="preserve"> voltage theoretical</t>
   </si>
   <si>
-    <t xml:space="preserve"> throttle value theoretical</t>
+    <t>Thottle guess</t>
   </si>
   <si>
-    <t>Thottle guess</t>
+    <t>servo setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> throttle value theoretical (4S battery)</t>
+  </si>
+  <si>
+    <t>throttle value 3S</t>
   </si>
 </sst>
 </file>
@@ -597,8 +603,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14561,16 +14568,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>255270</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>316230</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14875,20 +14882,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2182"/>
+  <dimension ref="A1:N2182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -14896,7 +14903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -14904,7 +14911,7 @@
         <v>14897</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -14912,7 +14919,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -14920,7 +14927,7 @@
         <v>9906.09</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -14928,7 +14935,7 @@
         <v>3045.46</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -14945,13 +14952,22 @@
         <v>12</v>
       </c>
       <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -14976,8 +14992,20 @@
       <c r="J9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <f>I9*180</f>
+        <v>48.540671382189231</v>
+      </c>
+      <c r="M9">
+        <f>I9/(3/4)</f>
+        <v>0.35956052875695727</v>
+      </c>
+      <c r="N9">
+        <f>M9*180</f>
+        <v>64.720895176252313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -15006,8 +15034,20 @@
       <c r="J10">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K19" si="2">I10*180</f>
+        <v>60.095383890720683</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M19" si="3">I10/(3/4)</f>
+        <v>0.44515099178311618</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:N19" si="4">M10*180</f>
+        <v>80.127178520960911</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -15022,7 +15062,7 @@
         <v>7019.8315789473681</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F17" si="2">E11-E10</f>
+        <f t="shared" ref="F11:F17" si="5">E11-E10</f>
         <v>850.03883283337836</v>
       </c>
       <c r="H11">
@@ -15036,8 +15076,20 @@
       <c r="J11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
+        <v>68.374982911825015</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.50648135490240753</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>91.166643882433362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -15052,7 +15104,7 @@
         <v>8094.8421052631575</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1075.0105263157893</v>
       </c>
       <c r="H12">
@@ -15066,8 +15118,20 @@
       <c r="J12">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <f t="shared" si="2"/>
+        <v>78.845864661654133</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.5840434419381787</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>105.12781954887217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -15082,7 +15146,7 @@
         <v>8981.4577114427866</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>886.61560617962914</v>
       </c>
       <c r="H13">
@@ -15096,8 +15160,20 @@
       <c r="J13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <f t="shared" si="2"/>
+        <v>87.481730955611553</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.64801282189341891</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>116.6423079408154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -15112,7 +15188,7 @@
         <v>9926.0102040816328</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>944.55249263884616</v>
       </c>
       <c r="H14">
@@ -15126,8 +15202,20 @@
       <c r="J14">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <f t="shared" si="2"/>
+        <v>96.681917572223711</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>0.71616235238684223</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>128.9092234296316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -15142,7 +15230,7 @@
         <v>10841.469072164948</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>915.45886808331488</v>
       </c>
       <c r="H15">
@@ -15156,8 +15244,20 @@
       <c r="J15">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <f t="shared" si="2"/>
+        <v>105.59872472887936</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>0.78221277576947668</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>140.7982996385058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -15172,7 +15272,7 @@
         <v>11856.6875</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1015.2184278350524</v>
       </c>
       <c r="H16">
@@ -15186,8 +15286,20 @@
       <c r="J16">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <f t="shared" si="2"/>
+        <v>115.48721590909091</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>0.85546085858585863</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>153.98295454545456</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -15202,7 +15314,7 @@
         <v>12681.48167539267</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>824.79417539266979</v>
       </c>
       <c r="H17">
@@ -15216,8 +15328,20 @@
       <c r="J17">
         <v>70</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <f t="shared" si="2"/>
+        <v>123.52092540966886</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>0.91496981784939901</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>164.69456721289183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -15246,8 +15370,20 @@
       <c r="J18">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <f t="shared" si="2"/>
+        <v>132.41594120165547</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>0.98085882371596655</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>176.55458826887397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>
@@ -15276,8 +15412,20 @@
       <c r="J19">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <f t="shared" si="2"/>
+        <v>138.94137622581499</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>1.0291953794504816</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>185.25516830108668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>13</v>
       </c>
@@ -15292,7 +15440,7 @@
         <v>956.79937423687443</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>14</v>
       </c>
@@ -15300,7 +15448,7 @@
         <v>4628</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>15</v>
       </c>
@@ -15311,7 +15459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>16</v>
       </c>
@@ -15322,7 +15470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>17</v>
       </c>
@@ -15330,7 +15478,7 @@
         <v>5108</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>18</v>
       </c>
@@ -15338,7 +15486,7 @@
         <v>4867</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>19</v>
       </c>
@@ -15346,7 +15494,7 @@
         <v>5101</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20</v>
       </c>
@@ -15354,7 +15502,7 @@
         <v>5101</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>21</v>
       </c>
@@ -15366,7 +15514,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>22</v>
       </c>
@@ -15374,7 +15522,7 @@
         <v>4950</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>23</v>
       </c>
@@ -15382,7 +15530,7 @@
         <v>4628</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>24</v>
       </c>
@@ -15390,7 +15538,7 @@
         <v>5711</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>25</v>
       </c>

</xml_diff>